<commit_message>
modified takscreenshot function in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Signature_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Signature_JS.xlsx
@@ -234,151 +234,6 @@
 validate1;
 link_Click(signature_test_link);
 validate2;
-SelectTestToRun(VT200_0876_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-DrawSignature(signature_view_xpath);
-TakeNativeScreenshot(VT200-0876);
-ClickNativeIcon(signature_ok_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0877_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-TakeNativeScreenshot(VT200-0877);
-ClickNativeIcon(signature_cancel_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0880_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-DrawSignature(signature_view_xpath);
-TakeNativeScreenshot(VT200-0880);
-ClickNativeIcon(signature_ok_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0881_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-DrawSignature(signature_view_xpath);
-TakeNativeScreenshot(VT200-0881-01);
-ClickNativeIcon(signature_ok_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-TakeNativeScreenshot(VT200-0881-02);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0885_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-Rotate_Screen(landscape);
-wait(2);
-TakeNativeScreenshot(VT200-0885);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0886_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-Rotate_Screen(landscape);
-wait(2);
-TakeNativeScreenshot(VT200-0886);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0887_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-DrawSignature(signature_view_xpath);
-TakeNativeScreenshot(VT200-0887-01);
-ClickNativeIcon(signature_clear_xpath);
-wait(2);
-TakeNativeScreenshot(VT200-0887-02);
-ClickNativeIcon(signature_ok_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0893_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-Rotate_Screen(landscape);
-wait(2);
-TakeNativeScreenshot(VT200-0893-01);
-wait(2);
-Rotate_Screen(potrait);
-wait(2);
-TakeNativeScreenshot(VT200-0893-02);
-wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
 SelectTestToRun(VT200_0878_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -439,22 +294,6 @@
 wait(4);
 TakeScreenshot(VT200-0879-02);
 wait(2);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signature_test_link);
-validate2;
-SelectTestToRun(VT200_0889_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-TakeNativeScreenshot(VT200-0889-01);
-Lock_UnlockScreen(lock);
-Lock_UnlockScreen(unlock);
-wait(2);
-TakeNativeScreenshot(VT200-0889-02);
 validate4;</t>
   </si>
   <si>
@@ -810,6 +649,167 @@
 ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
 PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0876_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+DrawSignature(signature_view_xpath);
+TakeScreenshot(VT200-0876);
+ClickNativeIcon(signature_ok_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0877_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+TakeScreenshot(VT200-0877);
+ClickNativeIcon(signature_cancel_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0880_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+DrawSignature(signature_view_xpath);
+TakeScreenshot(VT200-0880);
+ClickNativeIcon(signature_ok_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0881_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+DrawSignature(signature_view_xpath);
+TakeScreenshot(VT200-0881-01);
+ClickNativeIcon(signature_ok_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+TakeScreenshot(VT200-0881-02);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0885_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+Rotate_Screen(landscape);
+wait(2);
+TakeScreenshot(VT200-0885);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0886_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+Rotate_Screen(landscape);
+wait(2);
+TakeScreenshot(VT200-0886);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0887_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+DrawSignature(signature_view_xpath);
+TakeScreenshot(VT200-0887-01);
+ClickNativeIcon(signature_clear_xpath);
+wait(2);
+TakeScreenshot(VT200-0887-02);
+ClickNativeIcon(signature_ok_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0889_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+TakeScreenshot(VT200-0889-01);
+Lock_UnlockScreen(lock);
+Lock_UnlockScreen(unlock);
+wait(2);
+TakeScreenshot(VT200-0889-02);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(signature_test_link);
+validate2;
+SelectTestToRun(VT200_0893_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+Rotate_Screen(landscape);
+wait(2);
+TakeScreenshot(VT200-0893-01);
+wait(2);
+Rotate_Screen(potrait);
+wait(2);
+TakeScreenshot(VT200-0893-02);
+wait(2);
+validate4;</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +1402,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1464,13 +1464,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>68</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="2" t="s">
@@ -1497,10 +1497,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>21</v>
@@ -1551,10 +1551,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1578,10 +1578,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -1605,10 +1605,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="14"/>
@@ -1632,10 +1632,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="14"/>
@@ -1659,10 +1659,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="14"/>
@@ -1686,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="14"/>
@@ -1713,10 +1713,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="14"/>
@@ -1740,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>31</v>
@@ -1765,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>32</v>
@@ -1790,10 +1790,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="17"/>
@@ -1816,10 +1816,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="17"/>
@@ -1842,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I16" s="21"/>
     </row>
@@ -1867,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="I17" s="21"/>
     </row>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>34</v>
@@ -1917,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>35</v>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>36</v>

</xml_diff>